<commit_message>
added waits in login tests
</commit_message>
<xml_diff>
--- a/resources/web-data.xlsx
+++ b/resources/web-data.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>USERNAME</t>
   </si>
@@ -43,36 +42,6 @@
   </si>
   <si>
     <t>test3@gmail.com</t>
-  </si>
-  <si>
-    <t>test4@gmail.com</t>
-  </si>
-  <si>
-    <t>test5@gmail.com</t>
-  </si>
-  <si>
-    <t>test6@gmail.com</t>
-  </si>
-  <si>
-    <t>test7@gmail.com</t>
-  </si>
-  <si>
-    <t>test8@gmail.com</t>
-  </si>
-  <si>
-    <t>test9@gmail.com</t>
-  </si>
-  <si>
-    <t>test10@gmail.com</t>
-  </si>
-  <si>
-    <t>test11@gmail.com</t>
-  </si>
-  <si>
-    <t>raghava2706@gmail.com</t>
-  </si>
-  <si>
-    <t>training</t>
   </si>
 </sst>
 </file>
@@ -401,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,122 +414,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A12" r:id="rId2" display="test1@gmail.com"/>
+    <hyperlink ref="A3:A4" r:id="rId2" display="test1@gmail.com"/>
     <hyperlink ref="A3" r:id="rId3"/>
     <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A6" r:id="rId6"/>
-    <hyperlink ref="A7" r:id="rId7"/>
-    <hyperlink ref="A8" r:id="rId8"/>
-    <hyperlink ref="A9" r:id="rId9"/>
-    <hyperlink ref="A10" r:id="rId10"/>
-    <hyperlink ref="A11" r:id="rId11"/>
-    <hyperlink ref="A12" r:id="rId12"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="36" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
window handle and testng web update
</commit_message>
<xml_diff>
--- a/resources/web-data.xlsx
+++ b/resources/web-data.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5088" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="user" sheetId="2" r:id="rId2"/>
+    <sheet name="ppt" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>USERNAME</t>
   </si>
@@ -42,6 +44,24 @@
   </si>
   <si>
     <t>test3@gmail.com</t>
+  </si>
+  <si>
+    <t>raghava2706@gmail.com</t>
+  </si>
+  <si>
+    <t>training</t>
+  </si>
+  <si>
+    <t>PPT-NAME</t>
+  </si>
+  <si>
+    <t>PPT-PWD</t>
+  </si>
+  <si>
+    <t>whiteboxqa</t>
+  </si>
+  <si>
+    <t>SDLC - General</t>
   </si>
 </sst>
 </file>
@@ -372,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,4 +443,89 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>